<commit_message>
Costcode module in other setting 1. Insert/Update/Delete/Datatable 2. Donwload Import excel file 3. Import excel file 4. Export data in excel file
</commit_message>
<xml_diff>
--- a/invoice-frontend/src/assets/files/Costcode.xlsx
+++ b/invoice-frontend/src/assets/files/Costcode.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>cost_code</t>
   </si>
@@ -25,13 +25,10 @@
     <t>description</t>
   </si>
   <si>
-    <t>hemintest</t>
+    <t>testlast</t>
   </si>
   <si>
-    <t>hemnintest</t>
-  </si>
-  <si>
-    <t>testlast</t>
+    <t>SagarTest</t>
   </si>
 </sst>
 </file>
@@ -376,7 +373,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,24 +396,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>